<commit_message>
New 2016 wallet first release
</commit_message>
<xml_diff>
--- a/templates/month_template_2016.xlsx
+++ b/templates/month_template_2016.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yii\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\finances\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6405" windowHeight="11355"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6410" windowHeight="11360"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="2" r:id="rId1"/>
@@ -211,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -916,15 +916,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -934,19 +932,8 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -954,7 +941,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1311,12 +1298,69 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="57" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1326,137 +1370,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1775,39 +1759,39 @@
   </sheetPr>
   <dimension ref="B1:AA84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.42578125" customWidth="1"/>
+    <col min="1" max="1" width="1.453125" customWidth="1"/>
+    <col min="2" max="2" width="2.453125" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="4.1796875" customWidth="1"/>
+    <col min="6" max="6" width="7.1796875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" style="29" customWidth="1"/>
     <col min="9" max="9" width="8" style="17" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="25" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" style="25" customWidth="1"/>
+    <col min="11" max="11" width="7.7265625" customWidth="1"/>
     <col min="12" max="12" width="6" style="29" customWidth="1"/>
-    <col min="13" max="14" width="5.28515625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" style="17" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" style="21" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="17" customWidth="1"/>
-    <col min="18" max="18" width="30.28515625" style="25" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" style="17" customWidth="1"/>
-    <col min="20" max="20" width="28.42578125" style="17" customWidth="1"/>
-    <col min="21" max="21" width="1.7109375" customWidth="1"/>
-    <col min="22" max="22" width="1.85546875" customWidth="1"/>
-    <col min="23" max="23" width="8.42578125" customWidth="1"/>
-    <col min="24" max="25" width="7.85546875" customWidth="1"/>
-    <col min="26" max="26" width="2.42578125" customWidth="1"/>
+    <col min="13" max="14" width="5.26953125" style="29" customWidth="1"/>
+    <col min="15" max="15" width="7.26953125" style="17" customWidth="1"/>
+    <col min="16" max="16" width="22.453125" style="21" customWidth="1"/>
+    <col min="17" max="17" width="8.453125" style="17" customWidth="1"/>
+    <col min="18" max="18" width="30.26953125" style="25" customWidth="1"/>
+    <col min="19" max="19" width="7.81640625" style="17" customWidth="1"/>
+    <col min="20" max="20" width="28.453125" style="17" customWidth="1"/>
+    <col min="21" max="21" width="1.7265625" customWidth="1"/>
+    <col min="22" max="22" width="1.81640625" customWidth="1"/>
+    <col min="23" max="23" width="8.453125" customWidth="1"/>
+    <col min="24" max="25" width="7.81640625" customWidth="1"/>
+    <col min="26" max="26" width="2.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1835,7 +1819,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1863,7 +1847,7 @@
       <c r="Z2" s="9"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="4"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1891,17 +1875,17 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="146" t="s">
+      <c r="D4" s="178"/>
+      <c r="E4" s="179"/>
+      <c r="F4" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="148"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="164"/>
       <c r="J4" s="27"/>
       <c r="K4" s="49"/>
       <c r="L4" s="49"/>
@@ -1915,29 +1899,29 @@
       <c r="T4" s="49"/>
       <c r="U4" s="1"/>
       <c r="V4" s="112"/>
-      <c r="W4" s="172" t="s">
+      <c r="W4" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="178" t="s">
+      <c r="X4" s="142" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="140" t="s">
+      <c r="Y4" s="159" t="s">
         <v>9</v>
       </c>
       <c r="Z4" s="5"/>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="155" t="s">
+      <c r="D5" s="157" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="156"/>
-      <c r="F5" s="143"/>
-      <c r="G5" s="144"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="145"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="184"/>
+      <c r="H5" s="184"/>
+      <c r="I5" s="185"/>
       <c r="J5" s="109"/>
       <c r="K5" s="1"/>
       <c r="L5" s="49"/>
@@ -1951,20 +1935,20 @@
       <c r="T5" s="49"/>
       <c r="U5" s="1"/>
       <c r="V5" s="112"/>
-      <c r="W5" s="173"/>
-      <c r="X5" s="179"/>
-      <c r="Y5" s="141"/>
+      <c r="W5" s="182"/>
+      <c r="X5" s="143"/>
+      <c r="Y5" s="160"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="4"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="49"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="32"/>
       <c r="I6" s="19"/>
       <c r="J6" s="27"/>
       <c r="K6" s="1"/>
@@ -1979,47 +1963,47 @@
       <c r="T6" s="20"/>
       <c r="U6" s="1"/>
       <c r="V6" s="112"/>
-      <c r="W6" s="173"/>
-      <c r="X6" s="179"/>
-      <c r="Y6" s="141"/>
+      <c r="W6" s="182"/>
+      <c r="X6" s="143"/>
+      <c r="Y6" s="160"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="159"/>
-      <c r="F7" s="169" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="170"/>
-      <c r="H7" s="170"/>
-      <c r="I7" s="170"/>
-      <c r="J7" s="170"/>
-      <c r="K7" s="171"/>
-      <c r="L7" s="170" t="s">
+      <c r="D7" s="169"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="180" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="145" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="170"/>
-      <c r="N7" s="170"/>
-      <c r="O7" s="170"/>
-      <c r="P7" s="170"/>
-      <c r="Q7" s="170"/>
-      <c r="R7" s="170"/>
-      <c r="S7" s="171"/>
-      <c r="T7" s="183" t="s">
+      <c r="M7" s="145"/>
+      <c r="N7" s="145"/>
+      <c r="O7" s="145"/>
+      <c r="P7" s="145"/>
+      <c r="Q7" s="145"/>
+      <c r="R7" s="145"/>
+      <c r="S7" s="146"/>
+      <c r="T7" s="149" t="s">
         <v>21</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="112"/>
-      <c r="W7" s="173"/>
-      <c r="X7" s="179"/>
-      <c r="Y7" s="141"/>
+      <c r="W7" s="182"/>
+      <c r="X7" s="143"/>
+      <c r="Y7" s="160"/>
       <c r="Z7" s="5"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="4"/>
       <c r="C8" s="1"/>
       <c r="D8" s="40" t="s">
@@ -2028,17 +2012,17 @@
       <c r="E8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="155" t="s">
+      <c r="F8" s="157" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="156"/>
+      <c r="G8" s="158"/>
       <c r="H8" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="157" t="s">
+      <c r="I8" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="156"/>
+      <c r="J8" s="158"/>
       <c r="K8" s="7" t="s">
         <v>5</v>
       </c>
@@ -2051,27 +2035,27 @@
       <c r="N8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="181" t="s">
+      <c r="O8" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="182"/>
-      <c r="Q8" s="181" t="s">
+      <c r="P8" s="148"/>
+      <c r="Q8" s="147" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="182"/>
+      <c r="R8" s="148"/>
       <c r="S8" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="T8" s="184"/>
+      <c r="T8" s="150"/>
       <c r="U8" s="4"/>
       <c r="V8" s="112"/>
-      <c r="W8" s="174"/>
-      <c r="X8" s="180"/>
-      <c r="Y8" s="142"/>
+      <c r="W8" s="183"/>
+      <c r="X8" s="144"/>
+      <c r="Y8" s="161"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="1"/>
       <c r="D9" s="50"/>
@@ -2111,7 +2095,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="1"/>
       <c r="D10" s="78"/>
@@ -2151,7 +2135,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="1"/>
       <c r="D11" s="78"/>
@@ -2191,7 +2175,7 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="1"/>
       <c r="D12" s="87"/>
@@ -2208,7 +2192,7 @@
       <c r="L12" s="100"/>
       <c r="M12" s="65"/>
       <c r="N12" s="65"/>
-      <c r="O12" s="185"/>
+      <c r="O12" s="140"/>
       <c r="P12" s="64"/>
       <c r="Q12" s="105"/>
       <c r="R12" s="135"/>
@@ -2231,7 +2215,7 @@
       <c r="Z12" s="5"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="1"/>
       <c r="D13" s="81"/>
@@ -2271,7 +2255,7 @@
       <c r="Z13" s="5"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="1"/>
       <c r="D14" s="83"/>
@@ -2311,7 +2295,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="1"/>
       <c r="D15" s="83"/>
@@ -2351,7 +2335,7 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
       <c r="C16" s="1"/>
       <c r="D16" s="78"/>
@@ -2391,7 +2375,7 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="1"/>
       <c r="D17" s="81"/>
@@ -2431,7 +2415,7 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="1"/>
       <c r="D18" s="78"/>
@@ -2471,7 +2455,7 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="1"/>
       <c r="D19" s="87"/>
@@ -2511,7 +2495,7 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
       <c r="C20" s="1"/>
       <c r="D20" s="87"/>
@@ -2551,7 +2535,7 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
       <c r="C21" s="1"/>
       <c r="D21" s="81"/>
@@ -2591,7 +2575,7 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
       <c r="C22" s="1"/>
       <c r="D22" s="78"/>
@@ -2631,7 +2615,7 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="81"/>
@@ -2671,7 +2655,7 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="78"/>
@@ -2711,7 +2695,7 @@
       <c r="Z24" s="5"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="78"/>
@@ -2751,7 +2735,7 @@
       <c r="Z25" s="5"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="87"/>
@@ -2768,8 +2752,8 @@
       <c r="L26" s="103"/>
       <c r="M26" s="65"/>
       <c r="N26" s="65"/>
-      <c r="O26" s="185"/>
-      <c r="P26" s="186"/>
+      <c r="O26" s="140"/>
+      <c r="P26" s="141"/>
       <c r="Q26" s="105"/>
       <c r="R26" s="106"/>
       <c r="S26" s="130">
@@ -2791,7 +2775,7 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="1"/>
       <c r="D27" s="83"/>
@@ -2831,7 +2815,7 @@
       <c r="Z27" s="5"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
       <c r="C28" s="1"/>
       <c r="D28" s="78"/>
@@ -2871,7 +2855,7 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="1"/>
       <c r="D29" s="78"/>
@@ -2911,7 +2895,7 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
       <c r="C30" s="1"/>
       <c r="D30" s="81"/>
@@ -2951,7 +2935,7 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="1"/>
       <c r="D31" s="78"/>
@@ -2991,7 +2975,7 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="1"/>
       <c r="D32" s="78"/>
@@ -3031,7 +3015,7 @@
       <c r="Z32" s="5"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="1"/>
       <c r="D33" s="81"/>
@@ -3071,7 +3055,7 @@
       <c r="Z33" s="5"/>
       <c r="AA33" s="1"/>
     </row>
-    <row r="34" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="C34" s="1"/>
       <c r="D34" s="78"/>
@@ -3111,7 +3095,7 @@
       <c r="Z34" s="5"/>
       <c r="AA34" s="1"/>
     </row>
-    <row r="35" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
       <c r="C35" s="1"/>
       <c r="D35" s="81"/>
@@ -3151,7 +3135,7 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="1"/>
     </row>
-    <row r="36" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="4"/>
       <c r="C36" s="1"/>
       <c r="D36" s="78"/>
@@ -3191,7 +3175,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="1"/>
     </row>
-    <row r="37" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="4"/>
       <c r="C37" s="1"/>
       <c r="D37" s="78"/>
@@ -3231,7 +3215,7 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="1"/>
     </row>
-    <row r="38" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="4"/>
       <c r="C38" s="1"/>
       <c r="D38" s="81"/>
@@ -3271,7 +3255,7 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B39" s="4"/>
       <c r="C39" s="1"/>
       <c r="D39" s="86"/>
@@ -3311,27 +3295,27 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="4"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="165" t="s">
+      <c r="D40" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="166"/>
-      <c r="F40" s="164">
+      <c r="E40" s="177"/>
+      <c r="F40" s="175">
         <f>SUM(F9:F39)</f>
         <v>0</v>
       </c>
-      <c r="G40" s="163"/>
+      <c r="G40" s="174"/>
       <c r="H40" s="36">
         <f>SUM(H9:H39)</f>
         <v>0</v>
       </c>
-      <c r="I40" s="162">
+      <c r="I40" s="173">
         <f>SUM(I9:I39)</f>
         <v>0</v>
       </c>
-      <c r="J40" s="163"/>
+      <c r="J40" s="174"/>
       <c r="K40" s="35">
         <f>SUM(K9:K39)</f>
         <v>0</v>
@@ -3348,16 +3332,16 @@
         <f>SUM(N9:N39)</f>
         <v>0</v>
       </c>
-      <c r="O40" s="162">
+      <c r="O40" s="173">
         <f>SUM(O9:O39)</f>
         <v>0</v>
       </c>
-      <c r="P40" s="163"/>
-      <c r="Q40" s="160">
+      <c r="P40" s="174"/>
+      <c r="Q40" s="171">
         <f>SUM(Q9:Q39)</f>
         <v>0</v>
       </c>
-      <c r="R40" s="161"/>
+      <c r="R40" s="172"/>
       <c r="S40" s="35">
         <f>SUM(S9:S39)</f>
         <v>0</v>
@@ -3374,7 +3358,7 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="1"/>
     </row>
-    <row r="41" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B41" s="4"/>
       <c r="C41" s="1"/>
       <c r="D41" s="104"/>
@@ -3402,14 +3386,14 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="1"/>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B42" s="4"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="149" t="s">
+      <c r="D42" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="150"/>
-      <c r="F42" s="151"/>
+      <c r="E42" s="166"/>
+      <c r="F42" s="167"/>
       <c r="G42" s="110" t="str">
         <f>Y39</f>
         <v/>
@@ -3435,14 +3419,14 @@
       <c r="Z42" s="5"/>
       <c r="AA42" s="1"/>
     </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B43" s="4"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="152" t="s">
+      <c r="D43" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="153"/>
-      <c r="F43" s="154"/>
+      <c r="E43" s="152"/>
+      <c r="F43" s="153"/>
       <c r="G43" s="111">
         <f>K40</f>
         <v>0</v>
@@ -3468,14 +3452,14 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="1"/>
     </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B44" s="4"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="152" t="s">
+      <c r="D44" s="151" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="153"/>
-      <c r="F44" s="154"/>
+      <c r="E44" s="152"/>
+      <c r="F44" s="153"/>
       <c r="G44" s="111">
         <f>S40</f>
         <v>0</v>
@@ -3501,16 +3485,16 @@
       <c r="Z44" s="5"/>
       <c r="AA44" s="1"/>
     </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B45" s="4"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="152" t="s">
+      <c r="D45" s="151" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="153"/>
-      <c r="F45" s="154"/>
+      <c r="E45" s="152"/>
+      <c r="F45" s="153"/>
       <c r="G45" s="111">
-        <f>G43-G44</f>
+        <f>G47-G46</f>
         <v>0</v>
       </c>
       <c r="H45" s="48"/>
@@ -3534,17 +3518,17 @@
       <c r="Z45" s="5"/>
       <c r="AA45" s="1"/>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B46" s="4"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="152" t="s">
+      <c r="D46" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="153"/>
-      <c r="F46" s="154"/>
-      <c r="G46" s="111" t="str">
-        <f>IF(X39="","",F5)</f>
-        <v/>
+      <c r="E46" s="152"/>
+      <c r="F46" s="153"/>
+      <c r="G46" s="111">
+        <f>F5</f>
+        <v>0</v>
       </c>
       <c r="H46" s="48"/>
       <c r="I46" s="43"/>
@@ -3567,17 +3551,17 @@
       <c r="Z46" s="5"/>
       <c r="AA46" s="1"/>
     </row>
-    <row r="47" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B47" s="4"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="175" t="s">
+      <c r="D47" s="154" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="176"/>
-      <c r="F47" s="177"/>
-      <c r="G47" s="137" t="str">
-        <f>IF(X39="","",X39)</f>
-        <v/>
+      <c r="E47" s="155"/>
+      <c r="F47" s="156"/>
+      <c r="G47" s="137">
+        <f>X39</f>
+        <v>0</v>
       </c>
       <c r="H47" s="49"/>
       <c r="I47" s="19"/>
@@ -3600,7 +3584,7 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="1"/>
     </row>
-    <row r="48" spans="2:27" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:27" ht="9.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="4"/>
       <c r="C48" s="41"/>
       <c r="D48" s="1"/>
@@ -3628,7 +3612,7 @@
       <c r="Z48" s="5"/>
       <c r="AA48" s="1"/>
     </row>
-    <row r="49" spans="2:27" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:27" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B49" s="113"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -3656,7 +3640,7 @@
       <c r="Z49" s="10"/>
       <c r="AA49" s="1"/>
     </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -3682,7 +3666,7 @@
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
     </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -3708,7 +3692,7 @@
       <c r="X51" s="1"/>
       <c r="Y51" s="1"/>
     </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -3734,118 +3718,108 @@
       <c r="X52" s="1"/>
       <c r="Y52" s="1"/>
     </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
       <c r="R59" s="116"/>
     </row>
-    <row r="60" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B60" s="1"/>
       <c r="M60" s="117"/>
     </row>
-    <row r="61" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B62" s="1"/>
       <c r="J62" s="116"/>
       <c r="R62" s="117"/>
     </row>
-    <row r="63" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="X4:X8"/>
-    <mergeCell ref="L7:S7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D5:E5"/>
     <mergeCell ref="Y4:Y8"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="F4:I4"/>
@@ -3862,6 +3836,16 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="W4:W8"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="X4:X8"/>
+    <mergeCell ref="L7:S7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="T7:T8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="42" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>